<commit_message>
added more data visualization and random forest model for mental health prediction
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\youssefamr\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\youssefamr\Desktop\assistance system project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{DCAF2E05-595D-4D46-9638-338D4671C50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED4E298-9440-4626-8E7A-D609E5C032BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3986611F-C19C-4DA9-8254-50F015A96CBA}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{3986611F-C19C-4DA9-8254-50F015A96CBA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -4626,10 +4626,17 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -4655,8 +4662,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -4993,11 +5001,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EFBAD4F2-C6F0-465A-9BE5-E6D148BB805D}">
   <dimension ref="A1:N1500"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1447" workbookViewId="0">
-      <selection sqref="A1:N1500"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="4" max="4" width="21.7109375" customWidth="1"/>
+    <col min="5" max="5" width="16" customWidth="1"/>
+    <col min="6" max="6" width="15.5703125" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.85546875" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" customWidth="1"/>
+    <col min="12" max="12" width="20.140625" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="14" max="14" width="24" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -5062,7 +5083,7 @@
       <c r="F2">
         <v>0.68</v>
       </c>
-      <c r="G2">
+      <c r="G2" s="1">
         <v>12.36</v>
       </c>
       <c r="H2" t="s">
@@ -5071,7 +5092,7 @@
       <c r="I2" t="s">
         <v>17</v>
       </c>
-      <c r="J2">
+      <c r="J2" s="1">
         <v>8.01</v>
       </c>
       <c r="K2">
@@ -5766,7 +5787,7 @@
       <c r="F18">
         <v>4.76</v>
       </c>
-      <c r="G18">
+      <c r="G18" s="1">
         <v>11.4</v>
       </c>
       <c r="H18" t="s">
@@ -5775,7 +5796,7 @@
       <c r="I18" t="s">
         <v>24</v>
       </c>
-      <c r="J18">
+      <c r="J18" s="1">
         <v>4.62</v>
       </c>
       <c r="K18">
@@ -71001,5 +71022,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>